<commit_message>
Fixed Inventory minstick notification and returned crew remaining stick
</commit_message>
<xml_diff>
--- a/public/abcd/Schedule-wise EPKM Report.xlsx
+++ b/public/abcd/Schedule-wise EPKM Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>QixTix | Automated Fare Collection System</t>
   </si>
@@ -26,13 +26,13 @@
     <t>Depot : BALEWADI</t>
   </si>
   <si>
-    <t xml:space="preserve">Route : </t>
-  </si>
-  <si>
-    <t>From : 01-02-2019</t>
-  </si>
-  <si>
-    <t>To : 01-05-2019</t>
+    <t>Route : O2</t>
+  </si>
+  <si>
+    <t>From : 01-01-2019</t>
+  </si>
+  <si>
+    <t>To : 03-05-2019</t>
   </si>
   <si>
     <t>S. No</t>
@@ -68,10 +68,16 @@
     <t>ETM Passenger Count</t>
   </si>
   <si>
+    <t>O2-2-1</t>
+  </si>
+  <si>
+    <t>2:30 PM</t>
+  </si>
+  <si>
     <t>Print taken by : Satya</t>
   </si>
   <si>
-    <t>Print taken at : 01-05-2019 16:26:37</t>
+    <t>Print taken at : 03-05-2019 16:35:12</t>
   </si>
 </sst>
 </file>
@@ -496,10 +502,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -609,12 +615,47 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
-      <c r="A9" t="s">
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="C8" t="s">
         <v>18</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>13305</v>
+      </c>
+      <c r="G8">
+        <v>1234</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>-1234</v>
+      </c>
+      <c r="J8">
+        <v>221</v>
+      </c>
+      <c r="K8">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -627,8 +668,8 @@
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:H4"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="F9:K9"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="F10:K10"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>